<commit_message>
Add last checked to output
branch:
</commit_message>
<xml_diff>
--- a/tests/test_resources/test_namescan_explained.xlsx
+++ b/tests/test_resources/test_namescan_explained.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L71"/>
+  <dimension ref="A1:M71"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -464,20 +464,25 @@
       </c>
       <c r="I1" t="inlineStr">
         <is>
+          <t>LastChecked</t>
+        </is>
+      </c>
+      <c r="J1" t="inlineStr">
+        <is>
           <t>Matched</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>Verdict</t>
         </is>
       </c>
-      <c r="K1" t="inlineStr">
+      <c r="L1" t="inlineStr">
         <is>
           <t>Explanation</t>
         </is>
       </c>
-      <c r="L1" t="inlineStr">
+      <c r="M1" t="inlineStr">
         <is>
           <t>NeedExplanation</t>
         </is>
@@ -514,20 +519,25 @@
           <t>fded17b8481e0691f4a96e3af2938a41</t>
         </is>
       </c>
-      <c r="I2" t="b">
-        <v>1</v>
-      </c>
-      <c r="J2" t="inlineStr">
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J2" t="b">
+        <v>1</v>
+      </c>
+      <c r="K2" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K2" t="inlineStr">
+      <c r="L2" t="inlineStr">
         <is>
           <t>Mohammed Ali NASR: Not an Indonesian name: محمد علي نصر, Muhammad Ali Malkani: Politician, Muhammad Ali Malkani, male, born 1966-11-22 for Pakistan Peoples Party, Ali Nasir Muhammad: Not an Indonesian name: علي ناصر محمد, Muhammad Rapsel Ali: Politician, Muhammad Rapsel Ali, male, born 1971-05-06 for Nasdem Party, Muhammad Shujat Ali: Deceased 2007-04-01, Muhammad Yousuf Ali: Deceased 1998, Muhammad Ali Ridha: Politician, Muhammad Ali Ridha, male, born 1971-02-04 for Golongan Karya Party, Mohammed Ali NASR: Not an Indonesian name: محمد علي نصر, Muhammad Ali DURGHAM: Not an Indonesian name: محمد علي, Muhammad Ali DURGHAM: Not an Indonesian name: محمد علي, Muhammad Yusuf Ali: Deceased 1998-12-01, Iqbal Muhammad Ali Khan: Deceased 2022-04-19, Muhammad Alwi Dahlan: Politician, Muhammad Alwi Dahlan, male, born 1933-05-15, in Padang, Muhammad Unais Ali Hisyam: Politician, Muhammad Unais Ali Hisyam, male, born 1973-12-14, in , Muhammad Rudini Darwan Ali: Politician, Muhammad Rudini Darwan Ali, male, born 1986-05-09, Mohammad Ali Shah: Deceased 2013-02-04, Habib Muhammad Ali Al'habsyi: Politician, Habib Muhammad Ali Al'habsyi, male, born 1969-07-16, K.H. MUH. UNAIS ALI HISYAM, M.Pd.I: Public figure: Member of Dewan Perwakilan Rakyat (National Awakening Party Faction), Mohammad Ali JAFARI: Not an Indonesian name: محمد علي جعفري, Mohammad Ali Jinnah: Deceased 1948-09-11, ALI KONY: Public figure: Deputy, Lord’s Resistance Army, Mohammadian Abbas-Ali: Not an Indonesian name: Мохаммадян Аббас-Али, Abbas-Ali Mohammadian: Not an Indonesian name: عباسعلی محمدیان, Hodjatoleslam Ali KHAN MOHAMMADI: Not an Indonesian name: حجت الاسلام علی خان محمدی, Abbas-Ali MOHAMMADIAN: Not an Indonesian name: محمدیان عباس-علی, Ali Ahsan Mohammad Mojaheed: Deceased 2015-11-22</t>
         </is>
       </c>
-      <c r="L2" t="inlineStr">
+      <c r="M2" t="inlineStr">
         <is>
           <t>Ali Kony: Ali Kony is a Deputy in the Lord's Resistance Army (LRA) (CFe.002), a designated entity and the son of LRA leader Joseph Kony (CFi.009), a designated individual. Ali was incorporated into the LRA's leadership hierarchy in 2010.  He is part of a group of senior LRA officers who are based with Joseph Kony., Jafari Mohammad Ali: Foreign identifier: 28.
 Justification: Former Commander of the IRGC. Currently head of the Hazrat Baqiatollah al-Azam Cultural and Social Headquarters.
@@ -572,20 +582,25 @@
           <t>f4eb24399e2dc1183eba801996fe7c9f</t>
         </is>
       </c>
-      <c r="I3" t="b">
-        <v>1</v>
-      </c>
-      <c r="J3" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J3" t="b">
+        <v>1</v>
       </c>
       <c r="K3" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
           <t>Mohammed Bilal Brigadier General: Suspect in Syrian conflict, Mohammad Mufleh: Not an Indonesian name: محمد مفلح, Imad Mohammad Deeb Khamis: Not an Indonesian name: عماد محمد ديب خميس, Mohammad Abdul-Sattar Al Sayed Dr.: Not an Indonesian name: محمد عبد الستار السيد, Ahmad Ballul: Not an Indonesian name: أحمد بالول, Mohammed Ali Nasr General: Not an Indonesian name: محمد علي نصر, Amr Armanazi: Suspect in Syrian conflict, Mohammad Yahiya Moalla Dr.: Not an Indonesian name: محمد يحيى معلا, S. Muhammad: Politician, S. Muhammad, male, born 1960-04-25, in Gresik for National Awakening Party, Muhammed Zamrini Brigadier-General: Not an Indonesian name: محمد زمريني, Muhamad: Politician, Muhamad, male, born 1964-04-06, Muhammadong: Politician, Muhammadong, male, born 1969-01-09 for Great Indonesia Movement Party, Muhammad Yousef Hasouri Brigadier General: Not an Indonesian name: محمد يوسف حاصوري, Mohamad Ghazi Jalali: Suspect in Syrian conflict, Mohamed Heikmat Ibrahim: Not an Indonesian name: محمد حكمت إبراهيم, Mohamad Amer Mardini: Suspect in Syrian conflict, Muhammad Ali Durgham Major General: Not an Indonesian name: محمد علي, Jihad Mohamed Sultan Brigadier General: Not an Indonesian name: جهاد محمد سلطان, Mohammed Jabir: Not an Indonesian name: محمد جابر, Mohamed Maaruf Brigadier General: Not an Indonesian name: محمد معروف, Mohamad Fayez Barcha: Not an Indonesian name: محمد فايز برشة, Mohamed Khaddor Major General: Not an Indonesian name: محمد خضور, MuhammadAriLaw: Politician, Muhammad Ari Pratomo, male, born 1982-06-21</t>
         </is>
       </c>
-      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -618,20 +633,25 @@
           <t>d7216b875b45fff3aa6e9e02b8943644</t>
         </is>
       </c>
-      <c r="I4" t="b">
-        <v>1</v>
-      </c>
-      <c r="J4" t="inlineStr">
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J4" t="b">
+        <v>1</v>
+      </c>
+      <c r="K4" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K4" t="inlineStr">
+      <c r="L4" t="inlineStr">
         <is>
           <t>Abdul Aziz: Politician, Abdul Aziz, male, born 1969, Abdul Aziz: Deceased 1990-06-05, Abdul Aziz: Politician, Abdul Aziz, male, born 1972-10-12, Abdul Aziz: Politician, Abdul Aziz, male, born 1970-06-04, in Jakarta for United Development Party, H. ABDUL AZIZ, S.E.: Public figure: Member of Dewan Perwakilan Rakyat (United Development Party Faction), Abdul Azis Halid: Politician, Abdul Azis Halid, male, born 1968-11-25 for Golongan Karya Party, Abdul Azis Hasan: Politician, Abdul Azis Hasan, male, born 1967-06-30, in Ujung Pandang for People's Conscience Party, Abdul Azis Khafia: Politician, Abdul Azis Khafia, male, born 1975-11-23, Abdul Azis Suseno: Politician, Abdul Aziz Suseno, male, born 1965-05-10, in Blitar for Prosperous Justice Party, Sheikh Abdul Aziz: Deceased 2008-08-11, Abdul Aziz Abbasin: Not an Indonesian name: عبد العزيز عباسین, Abdul Aziz Angkat: Deceased 2009-02-03, Abdul Aziz Khandaker: Deceased 1991, Abdul Aziz Kamis: Politician, Abdul Aziz Kamis, male, born 1961-11-06, Abdul Aziz Mia: Politician, Abdul Aziz Mia, male, born 1955 for Bangladesh Jamaat-e-Islami, Abdul Aziz Junejo: Politician, Abdul Aziz Junejo, male, born 1961-12-07 for Pakistan Peoples Party, Aziz Abdullaev: Not an Indonesian name: Азиз Рефатович Абдуллаев, Dawood Ibrahim Kaskar: Foreigner: India</t>
         </is>
       </c>
-      <c r="L4" t="inlineStr">
+      <c r="M4" t="inlineStr">
         <is>
           <t>FAKER BEN ABDELAZZIZ BOUSSORA: Eyes: dark;
 Hair: black;
@@ -672,20 +692,25 @@
           <t>9df475a3b0b6446a32874fb3ab76f8fe</t>
         </is>
       </c>
-      <c r="I5" t="b">
-        <v>1</v>
-      </c>
-      <c r="J5" t="inlineStr">
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J5" t="b">
+        <v>1</v>
+      </c>
+      <c r="K5" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K5" t="inlineStr">
+      <c r="L5" t="inlineStr">
         <is>
           <t>Subhi Ahmad Al Abdallah: Not an Indonesian name: صبحي أحمد العبدالله, Khalaf Souleymane Abdallah: Suspect in Syrian conflict, Abdillah: Politician, Abdillah, male, born 1955-05-19, in Medan, Abdillah: Politician, Abdillah, male, born 1965-05-26, ABDALLAH: Suspect in Syrian conflict, Abdullah Berri: Not an Indonesian name: عبدالله بري, Abdullah Khaleel Hussein: Not an Indonesian name: عبدالله خليل حسين, Ali Abdullah Ayyub: Not an Indonesian name: علي عبدالله أيوب, MUSA HILAL ABDALLA ALNSIEM: Foreigner: Sudan, Edward Ğabdullacanof: Not an Indonesian name: Edvard Yunusovič, AL-ABDALLAH: Suspect in Syrian conflict, Suhail Al-Abdullah Brigadier General: Not an Indonesian name: سهيل العبدالله</t>
         </is>
       </c>
-      <c r="L5" t="inlineStr">
+      <c r="M5" t="inlineStr">
         <is>
           <t>Abdulla: Sheikh Tameem, born 2000-11-11, in , Pak Ud: Date of designation referred to in Article 7d(2)(i): 16.5.2005., Aris Sumarsono: Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 7 Jun. 2018. Review pursuant to Security Council resolution 2368 (2017) was concluded on 15 November 2021., ABDUL: (UK Sanctions List Ref):AQD0344. (UN Ref):QDi.187. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 7 Jun. 2018. Review pursuant to Security Council resolution 2368 (2017) was concluded on 15 November 2021. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/How-we-work/Notices/View-UN-Notices-Individuals
 Listed On: 18/05/2005;
@@ -733,20 +758,25 @@
           <t>72e0b290d121227107754fafe590387e</t>
         </is>
       </c>
-      <c r="I6" t="b">
-        <v>1</v>
-      </c>
-      <c r="J6" t="inlineStr">
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J6" t="b">
+        <v>1</v>
+      </c>
+      <c r="K6" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K6" t="inlineStr">
+      <c r="L6" t="inlineStr">
         <is>
           <t>Abu Bakar: Deceased 2019-07-13, Wan Abubakar: Politician, Wan Abu Bakar, male, born 1950-08-09, in Selat Panjang for National Mandate Party, Abu Bakar Abdi: Politician, Abu Bakar Abdi, male, born 1965-05-05, Abu Bakar Jamalia: Politician, Abu Bakar Jamalia, male, born 1953-07-21, in Kuala Tungkal, Abu Bakar Sidik: Politician, Abu Bakar Sidik, male, born 1962-05-25, Wan Abu Bakar: Politician, Wan Abu Bakar, male, born 1950-08-09 for National Mandate Party, Tagore Abubakar: Politician, Tagore Abu Bakar, male, born 1954-04-20, in Takengon for Indonesian Democratic Party – Struggle, Aboe Bakar Al-Habsyi: Politician, Aboe Bakar, Habib Aboe Bakar Alhabsyi, male, born 1964-10-15, in Jakarta for Prosperous Justice Party, Mohammed, Shariff Omar: Foreigner: TANZANIA, UNITED REPUBLIC OF, Abu Bakr Baira: Not an Indonesian name: أبو بكر مصطفى بعيرة</t>
         </is>
       </c>
-      <c r="L6" t="inlineStr">
+      <c r="M6" t="inlineStr">
         <is>
           <t>Abu Bakar Ba'asyir: Foreign identifier: QI.B.217.06.
 Sanctions: Art. 3 Abs. 1 und 2 (Finanzsanktionen) und Art. 4 sowie 4a (Ein- und Durchreiseverbot)
@@ -781,20 +811,25 @@
           <t>09c54507a4c070fc76c8a7f7fe300fc1</t>
         </is>
       </c>
-      <c r="I7" t="b">
-        <v>1</v>
-      </c>
-      <c r="J7" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J7" t="b">
+        <v>1</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L7" t="inlineStr">
+        <is>
           <t>Mohammad Mufleh: Not an Indonesian name: محمد مفلح, Imad Mohammad Deeb Khamis: Not an Indonesian name: عماد محمد ديب خميس, Mohammad Abdul-Sattar Al Sayed Dr.: Not an Indonesian name: محمد عبد الستار السيد, Ahmad Ballul: Not an Indonesian name: أحمد بالول, Mohammed Ali Nasr General: Not an Indonesian name: محمد علي نصر, Mohammad Yahiya Moalla Dr.: Not an Indonesian name: محمد يحيى معلا, Amr Armanazi: Suspect in Syrian conflict, Mohammed Bilal Brigadier General: Suspect in Syrian conflict, S. Muhammad: Politician, S. Muhammad, male, born 1960-04-25, in Gresik for National Awakening Party, Muhammed Zamrini Brigadier-General: Not an Indonesian name: محمد زمريني, Muhamad: Politician, Muhamad, male, born 1964-04-06, Muhammadong: Politician, Muhammadong, male, born 1969-01-09 for Great Indonesia Movement Party</t>
         </is>
       </c>
-      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -822,20 +857,25 @@
           <t>5c5076738ed3691b9b38c7eff1415b4d</t>
         </is>
       </c>
-      <c r="I8" t="b">
-        <v>1</v>
-      </c>
-      <c r="J8" t="inlineStr">
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J8" t="b">
+        <v>1</v>
+      </c>
+      <c r="K8" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K8" t="inlineStr">
+      <c r="L8" t="inlineStr">
         <is>
           <t>Ali Abdullah Ayyub: Not an Indonesian name: علي عبدالله أيوب, Abdullah Khaleel Hussein: Not an Indonesian name: عبدالله خليل حسين, Abdullah Berri: Not an Indonesian name: عبدالله بري, MUSA HILAL ABDALLA ALNSIEM: Foreigner: Sudan, ABDALLAH: Suspect in Syrian conflict, Abdillah: Politician, Abdillah, male, born 1965-05-26, Abdillah: Politician, Abdillah, male, born 1955-05-19, in Medan, Suhail Al-Abdullah Brigadier General: Not an Indonesian name: سهيل العبدالله, Subhi Ahmad Al Abdallah: Not an Indonesian name: صبحي أحمد العبدالله, Khalaf Souleymane Abdallah: Suspect in Syrian conflict, AL-ABDALLAH: Suspect in Syrian conflict</t>
         </is>
       </c>
-      <c r="L8" t="inlineStr">
+      <c r="M8" t="inlineStr">
         <is>
           <t xml:space="preserve">Abdulla: Sheikh Tameem, born 2000-11-11, in </t>
         </is>
@@ -867,20 +907,25 @@
           <t>4912713fed5d8960f4e2f2f31c606c5e</t>
         </is>
       </c>
-      <c r="I9" t="b">
-        <v>1</v>
-      </c>
-      <c r="J9" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J9" t="b">
+        <v>1</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L9" t="inlineStr">
+        <is>
           <t>Suhayl Hassan: Suspect in Syrian conflict, Malik Hasan: Not an Indonesian name: مالك حسن, Hossein Taeb: Not an Indonesian name: حسين طائب, M. M. Hassan: Foreigner: British Raj; Dominion of India; India, Hasani: Deceased 2018-02-17, Bassam Al Hassan: Not an Indonesian name: بسام الحسن, Ibrahim Al-Hassan Major General: Not an Indonesian name: إبراهيم الحسن, AL-HASAN: Suspect in Syrian conflict, Jamil Hassan: Not an Indonesian name: جميل حسن, Nabil Al-Hasan: Not an Indonesian name: نبيل الحسن, Nabil AL-HASAN: Not an Indonesian name: حسن نبيل, Ahmed Mahmoud Hassan: Not an Indonesian name: šejk Hassan, Hassan Khan: Foreigner: India; British Raj; Dominion of India</t>
         </is>
       </c>
-      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -908,20 +953,25 @@
           <t>09540d816c7e95a40da8678fb05429a8</t>
         </is>
       </c>
-      <c r="I10" t="b">
-        <v>1</v>
-      </c>
-      <c r="J10" t="inlineStr">
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J10" t="b">
+        <v>1</v>
+      </c>
+      <c r="K10" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K10" t="inlineStr">
+      <c r="L10" t="inlineStr">
         <is>
           <t>Ahmed Khalil Khalil: Not an Indonesian name: احمد خليل خليل, Ahmed al-Jarroucheh Major General: Not an Indonesian name: أحمد الجاروشة, Ahmed Dibe: Not an Indonesian name: أحمد ديب, Ghassan Ahmed Ghannam: Suspect in Syrian conflict, Ahmad Tohari: Politician, Ahmad, male, born 1948-06-13, in , Ahmad: Politician, Ahmad, male, born 1966-11-27, Jawdat al-Ahmed Brigadier General: Not an Indonesian name: جودت الأحمد, Mohammed al-Ahmed: Not an Indonesian name: محمد الأحمد, Ahmad Sayyed: Not an Indonesian name: أحمد السيد, Riad al-Ahmed Major General: Not an Indonesian name: رياض الأحمد, Ahmad AL-SAYED: Suspect in Syrian conflict</t>
         </is>
       </c>
-      <c r="L10" t="inlineStr">
+      <c r="M10" t="inlineStr">
         <is>
           <t>Khalil Yusif HARB: Sayyid AHMAD, Abu MUSTAFA, Mustafa Khalil HARB, Khalil Yusuf HARB, Hajj Ya'taqad Khalil HARB, born 09 Oct 1958</t>
         </is>
@@ -963,20 +1013,25 @@
           <t>3de6ddb729214127897b5c88f532f95c</t>
         </is>
       </c>
-      <c r="I11" t="b">
-        <v>1</v>
-      </c>
-      <c r="J11" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I11" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J11" t="b">
+        <v>1</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L11" t="inlineStr">
+        <is>
           <t>أحمد الشيخ عبدالقادر: Not an Indonesian name: أحمد الشيخ عبدالقادر, Ahmad al-Sheik ABDULQADER: Not an Indonesian name: القادر عبد الشيخ أحمد, Ahmad al-Sheik Abdulquader: Not an Indonesian name: أحمد الشيخ عبدالقادر, Abdul Razak Ahmad: Deceased 2007, Ahmad Mufti Salim: Politician, Ahmad Mufti Salim, male, born 1975-08-28, Subhi Ahmad AL ABDALLAH: Not an Indonesian name: صبحي احمد العبدالله, Subhi Ahmad Al-Abdullah: Suspect in Syrian conflict, Subhi Ahmad AL ABDALLAH: Not an Indonesian name: صبحي احمد العبدالله</t>
         </is>
       </c>
-      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1004,20 +1059,25 @@
           <t>49d7419d2480eed4d2bd7c94d7c09bef</t>
         </is>
       </c>
-      <c r="I12" t="b">
-        <v>1</v>
-      </c>
-      <c r="J12" t="inlineStr">
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J12" t="b">
+        <v>1</v>
+      </c>
+      <c r="K12" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K12" t="inlineStr">
+      <c r="L12" t="inlineStr">
         <is>
           <t>Hussein Mahmoud Farzat: Not an Indonesian name: حسين محمود فرزات, Makhmoud Al-Khattib: Not an Indonesian name: محمود الخطيب</t>
         </is>
       </c>
-      <c r="L12" t="inlineStr">
+      <c r="M12" t="inlineStr">
         <is>
           <t>Yassin SYAWAL: Associated With: Al Qaeda;
 NZ Designation Date: 1/21/2004;
@@ -1063,20 +1123,25 @@
           <t>253428caaa71a1b6ab4c039e0c36537c</t>
         </is>
       </c>
-      <c r="I13" t="b">
-        <v>1</v>
-      </c>
-      <c r="J13" t="inlineStr">
+      <c r="I13" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J13" t="b">
+        <v>1</v>
+      </c>
+      <c r="K13" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K13" t="inlineStr">
+      <c r="L13" t="inlineStr">
         <is>
           <t>Ahmad Farhan Hamid: Politician, Ahmad Farhan Hamid, male, born 1953-01-21 for National Mandate Party, Hamid Reza EMADI: Public figure: Former Press TV Newsroom Director. Former Press TV Senior Producer., Fathi Ahmad Hammad: Politician, Fathi Ahmad Hammad, male, born 1961, Najm Hamad AL AHMAD: Not an Indonesian name: نجم حمد الأحمد, Najm Hamad Al Ahmad: Suspect in Syrian conflict, Najm Hamad Al Ahmad: Not an Indonesian name: نجم حمد الأحمد, Najm Hamad AL AHMAD: Not an Indonesian name: نجم حمد الأحمد</t>
         </is>
       </c>
-      <c r="L13" t="inlineStr">
+      <c r="M13" t="inlineStr">
         <is>
           <t xml:space="preserve">Fathi Ahmad Mohammad HAMMAD: Fathi Ahmad HAMMAD, Fathy Ahmed HAMAD, Fathi HAMAD, born 1961, in , Fathi Ahmad Mohammad HAMMAD: Fathi Ahmad HAMMAD, Fathy Ahmed HAMAD, Fathi HAMAD, born 1961, in </t>
         </is>
@@ -1108,20 +1173,25 @@
           <t>df42a8a1b3c158561d1977664571ed5f</t>
         </is>
       </c>
-      <c r="I14" t="b">
-        <v>1</v>
-      </c>
-      <c r="J14" t="inlineStr">
+      <c r="I14" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J14" t="b">
+        <v>1</v>
+      </c>
+      <c r="K14" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K14" t="inlineStr">
+      <c r="L14" t="inlineStr">
         <is>
           <t>Abdurrahman B.T.M: Politician, Abdurrahman B.T.M, male, born 1962-06-19, Abdurachman: Politician, Abdurachman, male, born 1954-02-05 for Perindo Party</t>
         </is>
       </c>
-      <c r="L14" t="inlineStr">
+      <c r="M14" t="inlineStr">
         <is>
           <t>Pak Ud: Date of designation referred to in Article 7d(2)(i): 16.5.2005., Aris Sumarsono: Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 7 Jun. 2018. Review pursuant to Security Council resolution 2368 (2017) was concluded on 15 November 2021., ABDUL: (UK Sanctions List Ref):AQD0344. (UN Ref):QDi.187. Review pursuant to Security Council resolution 1822 (2008) was concluded on 8 Jun. 2010. Review pursuant to Security Council resolution 2253 (2015) was concluded on 7 Jun. 2018. Review pursuant to Security Council resolution 2368 (2017) was concluded on 15 November 2021. INTERPOL-UN Security Council Special Notice web link: https://www.interpol.int/en/How-we-work/Notices/View-UN-Notices-Individuals
 Listed On: 18/05/2005;
@@ -1160,20 +1230,25 @@
           <t>8a59047775ebb86b1dda2e11dbe5bda5</t>
         </is>
       </c>
-      <c r="I15" t="b">
-        <v>1</v>
-      </c>
-      <c r="J15" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I15" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J15" t="b">
+        <v>1</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L15" t="inlineStr">
+        <is>
           <t>Mohammad Hatta: Deceased 1980-03-14, Muhammad Hatta: Politician, Muhammad Hatta, male, born 1973-08-17, in Surakarta, MOHAMMAD HATTA: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction), Hatta Rajasa: Politician, Ir. M. Hatta Rajasa, Muhammad Hatta Rajasa, male, born 1953-09-18, in Palembang for National Mandate Party, Mohammad Hatta: Politician, Mohammad Hatta, male, born 1973-08-17, in Surabaya for National Mandate Party, Rana Muhammad Hayat: Politician, Rana Muhammad Hayat Khan, male, born 1955-12-24 for Pakistan Muslim League (N), Muhammad Hadi Nasrallah: Deceased 1997, Mian Muhammad Akhtar Hayat: Politician, Mian Muhammad Akhtar Hayat, male, born 1950 for Pakistan Tehreek-e-Insaf</t>
         </is>
       </c>
-      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -1206,20 +1281,25 @@
           <t>75808479305f79406bf05066f6b9b218</t>
         </is>
       </c>
-      <c r="I16" t="b">
-        <v>1</v>
-      </c>
-      <c r="J16" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I16" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J16" t="b">
+        <v>1</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L16" t="inlineStr">
+        <is>
           <t>Ruslan Abdul Gani: Politician, Ruslan Abdul Gani, male, born 1958-12-09 for People's Conscience Party, Abdul Ghani Lone: Deceased 2002-05-21, Rusmin Abdul Gani: Politician, Rusmin Abdul Gani, male, born 1980-12-08, Emad Abdul-Ghani Sabouni: Not an Indonesian name: عماد عبدالغني صابوني, Abdul Ganie Mohamed: Politician, Abdul Ganie Mohamed, male, born 1937-11-04, Abdul Ghani Kasuba: Politician, Abdul Ghani Kasuba, male, born 1951-12-21, in Bacan islands for Prosperous Justice Party, Abdul Ghani Baradar: Foreigner: Afghanistan; Democratic Republic of Afghanistan; Islamic State of Afghanistan; Kingdom of Afghanistan; Republic of Afghanistan</t>
         </is>
       </c>
-      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -1252,20 +1332,25 @@
           <t>bb84b1fecd2136ccc4d444541af8f375</t>
         </is>
       </c>
-      <c r="I17" t="b">
-        <v>1</v>
-      </c>
-      <c r="J17" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I17" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J17" t="b">
+        <v>1</v>
       </c>
       <c r="K17" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L17" t="inlineStr">
+        <is>
           <t>Abd Allah Mohamed Ragab Abdel Rahman: Foreigner: Egyptian, Karimi Ahmad Hasan: Not an Indonesian name: Карими Ахмад Хасан, Ahmed Salem HASSAN: Suspect in Syrian conflict, Michel KASSOUHA: Not an Indonesian name: ميشال كسوحة, Michel Kassouha: Suspect in Syrian conflict, Michel KASSOUHA: Not an Indonesian name: ميشال كسوحة, Ahmed Mahmoud Hassan: Not an Indonesian name: šejk Hassan</t>
         </is>
       </c>
-      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -1298,20 +1383,25 @@
           <t>397c05eb1ba3df6abd492197963d851d</t>
         </is>
       </c>
-      <c r="I18" t="b">
-        <v>1</v>
-      </c>
-      <c r="J18" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I18" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J18" t="b">
+        <v>1</v>
       </c>
       <c r="K18" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L18" t="inlineStr">
+        <is>
           <t>Ibrahim AL-HASSAN: Not an Indonesian name: ابراهيم الحسن, Ibrahim AL-HASSAN: Not an Indonesian name: ابراهيم الحسن, Ibrahim Al-Hassan: Suspect in Syrian conflict, AL-HASAN: Suspect in Syrian conflict, Ibrahim Al-Hassan Major General: Not an Indonesian name: إبراهيم الحسن, Dawood Ibrahim Kaskar: Foreigner: India</t>
         </is>
       </c>
-      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -1339,20 +1429,25 @@
           <t>8ffb8c628b01d484f9b330128fab795d</t>
         </is>
       </c>
-      <c r="I19" t="b">
-        <v>1</v>
-      </c>
-      <c r="J19" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I19" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J19" t="b">
+        <v>1</v>
       </c>
       <c r="K19" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
           <t>Mulyadi: Politician, Mulyadi, male, born 1963-02-13, in Bukittinggi for Democratic Party, Mulyadi: Politician, Mulyadi, male, born 1967-05-14, in Jakarta for United Development Party, Mulyadi: Politician, Mulyadi, male, born 1970-03-01, Mulyadi: Politician, Mulyadi, male, born 1970-11-02, in Bogor for Great Indonesia Movement Party, Ir. H. MULYADI: Public figure: Member of Dewan Perwakilan Rakyat (Democrat Party Faction), Muliadi: Politician, Muliadi, male, born 1970-07-07</t>
         </is>
       </c>
-      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -1380,20 +1475,25 @@
           <t>6d21e48aeddfc7669ef3f2fc66bd08ad</t>
         </is>
       </c>
-      <c r="I20" t="b">
-        <v>1</v>
-      </c>
-      <c r="J20" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I20" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J20" t="b">
+        <v>1</v>
       </c>
       <c r="K20" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L20" t="inlineStr">
+        <is>
           <t>Amar Ismael: Not an Indonesian name: عمار إسماعيل, Ismael Ismael: Suspect in Syrian conflict, Ezzedine Ismael: Not an Indonesian name: عزالدين إسماعيل, Ismail: Politician, Ismail, male, born 1957-05-19, M. M. Ismail: Deceased 2005-01-17</t>
         </is>
       </c>
-      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -1421,20 +1521,25 @@
           <t>7c3a99404c8ea3b3ac294564aa6a5dd7</t>
         </is>
       </c>
-      <c r="I21" t="b">
-        <v>1</v>
-      </c>
-      <c r="J21" t="inlineStr">
+      <c r="I21" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K21" t="inlineStr">
+      <c r="L21" t="inlineStr">
         <is>
           <t>Ali Barakat: Not an Indonesian name: علي بركات, Ali: Politician, Ali, male, born 1950-09-01, Nasser Al-Ali Brigadier General: Not an Indonesian name: ناصر العلي, Aous "Ali" Aslan Major General: Not an Indonesian name: أوس "</t>
         </is>
       </c>
-      <c r="L21" t="inlineStr">
+      <c r="M21" t="inlineStr">
         <is>
           <t>Ahmad Al Ghazali: Al, Ahmad Al Ghazali Köhler, Al Ghazali, male, born 1997-09-01, in Jakarta</t>
         </is>
@@ -1466,20 +1571,25 @@
           <t>40508c9f66b41d3eb6420add757b1693</t>
         </is>
       </c>
-      <c r="I22" t="b">
-        <v>1</v>
-      </c>
-      <c r="J22" t="inlineStr">
+      <c r="I22" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J22" t="b">
+        <v>1</v>
+      </c>
+      <c r="K22" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K22" t="inlineStr">
+      <c r="L22" t="inlineStr">
         <is>
           <t>Ali Barakat: Not an Indonesian name: علي بركات, Ali: Politician, Ali, male, born 1950-09-01, Nasser Al-Ali Brigadier General: Not an Indonesian name: ناصر العلي, Aous "Ali" Aslan Major General: Not an Indonesian name: أوس "</t>
         </is>
       </c>
-      <c r="L22" t="inlineStr">
+      <c r="M22" t="inlineStr">
         <is>
           <t>Ahmad Al Ghazali: Al, Ahmad Al Ghazali Köhler, Al Ghazali, male, born 1997-09-01, in Jakarta</t>
         </is>
@@ -1511,20 +1621,25 @@
           <t>25eef2c7bdb80105d487da5da31373d7</t>
         </is>
       </c>
-      <c r="I23" t="b">
-        <v>1</v>
-      </c>
-      <c r="J23" t="inlineStr">
+      <c r="I23" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J23" t="b">
+        <v>1</v>
+      </c>
+      <c r="K23" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K23" t="inlineStr">
+      <c r="L23" t="inlineStr">
         <is>
           <t>Mat Solar: Politician, Nasrullah, male, born 1962-12-04, in Jakarta for United Development Party, Nasrullah: Politician, Nasrullah, male, born 1968-11-18, in Pekalongan for National Mandate Party, Nasrul: Politician, Nasrul, male, born 1967-05-14, Nasrullo Sayidov: Politician, Nasrullo Sayyid), male, born 1958-02-20</t>
         </is>
       </c>
-      <c r="L23" t="inlineStr">
+      <c r="M23" t="inlineStr">
         <is>
           <t>Nasrullah KHAN: Court: Manchester;
 Offence: Drugs Class A;
@@ -1565,20 +1680,25 @@
           <t>80816fe9feef2412377504494d78b701</t>
         </is>
       </c>
-      <c r="I24" t="b">
-        <v>1</v>
-      </c>
-      <c r="J24" t="inlineStr">
+      <c r="I24" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+      <c r="K24" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K24" t="inlineStr">
+      <c r="L24" t="inlineStr">
         <is>
           <t>A. Rahman: Politician, A. Rahman, male, born 1959-02-17 for United Development Party, Rahman: Politician, Rahman, male, born 1962-01-30, in Bandung for United Development Party, K. Rahman Khan: Foreigner: India; British Raj; Dominion of India, B. Raman: Deceased 2013-06-16</t>
         </is>
       </c>
-      <c r="L24" t="inlineStr">
+      <c r="M24" t="inlineStr">
         <is>
           <t>MR. K.M. RAHMAN: Ineligibility Period: From 2011-07-29 To 2999-12-31
 Ineligibility Reason: Consultant Guidelines 1.25(a)(ii)
@@ -1613,20 +1733,25 @@
           <t>e9023e3c3a12dffe1e5e3db009ebba0c</t>
         </is>
       </c>
-      <c r="I25" t="b">
-        <v>1</v>
-      </c>
-      <c r="J25" t="inlineStr">
+      <c r="I25" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J25" t="b">
+        <v>1</v>
+      </c>
+      <c r="K25" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K25" t="inlineStr">
+      <c r="L25" t="inlineStr">
         <is>
           <t>Anwar: Politician, Anwar, male, born 1965-08-05, Anwar: Politician, Anwar, male, born 1963-08-06, M.K. Anwar: Deceased 2017-10-24</t>
         </is>
       </c>
-      <c r="L25" t="inlineStr">
+      <c r="M25" t="inlineStr">
         <is>
           <t>SHAIKH, ANWAR: Reason: Wanted By India;
 Language Spoken: English, Hindi, Urdu;
@@ -1660,20 +1785,25 @@
           <t>64b7f9201a6f2bf167bb502a74d5918f</t>
         </is>
       </c>
-      <c r="I26" t="b">
-        <v>1</v>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I26" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
       </c>
       <c r="K26" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L26" t="inlineStr">
+        <is>
           <t>Amer al-Achi Major General: Not an Indonesian name: عامر العشي, Mahmoud Ibraheem Sa’iid Dr.: Not an Indonesian name: محمود ابراهيم سعيد, B. Ibrahim: Politician, B. Ibrahim, male, born 1946-01-02, Mohammed Ibrahim: Politician, Moh.Ibrahim, male, born 1936</t>
         </is>
       </c>
-      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -1701,20 +1831,25 @@
           <t>b3dcd391162c5bab4b2fb749531731bf</t>
         </is>
       </c>
-      <c r="I27" t="b">
-        <v>1</v>
-      </c>
-      <c r="J27" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I27" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J27" t="b">
+        <v>1</v>
       </c>
       <c r="K27" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L27" t="inlineStr">
+        <is>
           <t>Samsudin: Politician, Samsudin, male, born 1962-12-01, Samsudin S.: Politician, Samsudin S., male, born 1982-02-12, Syamsudin: Politician, Syamsudin, male, born 1954-02-07, Syamsuddin Hb.: Politician, Syamsuddin Hb., male, born 1974-07-07 for Nasdem Party</t>
         </is>
       </c>
-      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -1742,20 +1877,25 @@
           <t>2af9fb8e197632fb665fad996c0bd112</t>
         </is>
       </c>
-      <c r="I28" t="b">
-        <v>1</v>
-      </c>
-      <c r="J28" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I28" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J28" t="b">
+        <v>1</v>
       </c>
       <c r="K28" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L28" t="inlineStr">
+        <is>
           <t>R. Sudirman: Politician, R. Sudirman, male, born 1957-12-30, in Maros for Nasdem Party, Sudirman: Politician, Sudirman, male, born 1974-11-10, Sudirman: Politician, Sudirman, male, born 1979-10-28, Sudarmanto: Politician, Sudarmanto, male, born 1957-05-15 for Great Indonesia Movement Party</t>
         </is>
       </c>
-      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -1783,20 +1923,25 @@
           <t>5f24ef0ec08fb05c99e7b7034c20f514</t>
         </is>
       </c>
-      <c r="I29" t="b">
-        <v>1</v>
-      </c>
-      <c r="J29" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I29" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J29" t="b">
+        <v>1</v>
       </c>
       <c r="K29" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L29" t="inlineStr">
+        <is>
           <t>Sukiman: Politician, Sukiman, male, born 1953-08-10, Sukiman: Politician, Sukiman, male, born 1968-07-15, in Nanga Pak for National Mandate Party, Sukiman: Politician, Sukiman, male, born 1953-08-10, in Madiun, H. SUKIMAN, S. Pd., M.M.: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction)</t>
         </is>
       </c>
-      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -1824,20 +1969,25 @@
           <t>333ff192568bbc2510c816314b1e2754</t>
         </is>
       </c>
-      <c r="I30" t="b">
-        <v>1</v>
-      </c>
-      <c r="J30" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I30" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J30" t="b">
+        <v>1</v>
       </c>
       <c r="K30" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L30" t="inlineStr">
+        <is>
           <t>Syamsudin: Politician, Syamsudin, male, born 1954-02-07, Syamsuddin Hb.: Politician, Syamsuddin Hb., male, born 1974-07-07 for Nasdem Party, Samsudin: Politician, Samsudin, male, born 1962-12-01, Samsudin S.: Politician, Samsudin S., male, born 1982-02-12</t>
         </is>
       </c>
-      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -1870,20 +2020,25 @@
           <t>20ea551df76220dea8c0b309cc217c1c</t>
         </is>
       </c>
-      <c r="I31" t="b">
-        <v>1</v>
-      </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J31" t="b">
+        <v>1</v>
       </c>
       <c r="K31" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
           <t>Abdul Haris: Politician, Abdul Haris, male, born 1956-07-11, Abdul Haris: Politician, Abdul Haris, male, born 1968-05-03, Abdul Haris Makkie: Politician, Abdul Haris Makkie, male, born 1962-05-10</t>
         </is>
       </c>
-      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -1921,20 +2076,25 @@
           <t>08644320a4caafa74f5970cea88314ab</t>
         </is>
       </c>
-      <c r="I32" t="b">
-        <v>1</v>
-      </c>
-      <c r="J32" t="inlineStr">
+      <c r="I32" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J32" t="b">
+        <v>1</v>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K32" t="inlineStr">
+      <c r="L32" t="inlineStr">
         <is>
           <t>Sri Oetari Ratna Dewi: Deceased 2003-11-01, Ratna Juwita Sari: Politician, Ratna Juwita Sari, female, born 1984-03-29, in Tuban for National Awakening Party, Dr. Ratna De: Politician, Dr. Ratna De, female, born 1948-09-06, Ratna Sarah Ayu: Politician, Ratna Sarah Ayu, female, born 1974-09-05, in Jakarta for National Mandate Party</t>
         </is>
       </c>
-      <c r="L32" t="inlineStr">
+      <c r="M32" t="inlineStr">
         <is>
           <t>Dewi Sukarno: Naoko Nemoto, Ratna Sari Dewi Sukarno, female, born 1940-02-06, in Tokyo</t>
         </is>
@@ -1966,20 +2126,25 @@
           <t>efa685dc42d83a773ede4293f84ecce8</t>
         </is>
       </c>
-      <c r="I33" t="b">
-        <v>1</v>
-      </c>
-      <c r="J33" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J33" t="b">
+        <v>1</v>
       </c>
       <c r="K33" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L33" t="inlineStr">
+        <is>
           <t>Firmandez: Politician, Firmandez, male, born 1960-10-21, in Banda Aceh for Golongan Karya Party, H. FIRMANDEZ: Public figure: Member of Dewan Perwakilan Rakyat (Golkar Party Faction), Firmansyah: Politician, Firmansyah, male, born 1966-03-11</t>
         </is>
       </c>
-      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -2007,20 +2172,25 @@
           <t>4ca30ebddb71a501bd9cd8fae823b1f1</t>
         </is>
       </c>
-      <c r="I34" t="b">
-        <v>1</v>
-      </c>
-      <c r="J34" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J34" t="b">
+        <v>1</v>
       </c>
       <c r="K34" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L34" t="inlineStr">
+        <is>
           <t>Haerudin: Politician, Haerudin, male, born 1974-05-28, in Garut for Crescent Star Party, HAERUDIN, S.Ag, MH: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction), Hairudin: Politician, Hairudin, male, born 1967-10-07 for Great Indonesia Movement Party</t>
         </is>
       </c>
-      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -2048,20 +2218,25 @@
           <t>68eacd6aba029572f084c603e329e1db</t>
         </is>
       </c>
-      <c r="I35" t="b">
-        <v>1</v>
-      </c>
-      <c r="J35" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J35" t="b">
+        <v>1</v>
       </c>
       <c r="K35" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L35" t="inlineStr">
+        <is>
           <t>Imran: Deceased 2020-03-28, Amran: Politician, Amran, male, born 1968-07-18, in  for National Mandate Party, AMRAN, S.E.: Public figure: Member of Dewan Perwakilan Rakyat (National Mandate Party Faction)</t>
         </is>
       </c>
-      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -2094,20 +2269,25 @@
           <t>05d2804cbc84f1ed167edee8e9ae4467</t>
         </is>
       </c>
-      <c r="I36" t="b">
-        <v>1</v>
-      </c>
-      <c r="J36" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J36" t="b">
+        <v>1</v>
       </c>
       <c r="K36" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L36" t="inlineStr">
+        <is>
           <t>M. Nasir: Politician, M. Nasir, male, born 1973-03-19, Nasir Khan: Politician, Nasir Khan Khattak, male, born 1966-02-09, Nasir Khan: Deceased 1974-05-03</t>
         </is>
       </c>
-      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -2135,20 +2315,25 @@
           <t>cfcfe0661539647591a2e4df365a7f18</t>
         </is>
       </c>
-      <c r="I37" t="b">
-        <v>1</v>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J37" t="b">
+        <v>1</v>
       </c>
       <c r="K37" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L37" t="inlineStr">
+        <is>
           <t>Mardani: Politician, Mardani, born 1968-04-09 for Prosperous Justice Party, Mardani Ali Sera: Politician, Mardani, male, born 1968-04-09, in Jakarta for Prosperous Justice Party, Dr. H. MARDANI, M.Eng.: Public figure: Member of Dewan Perwakilan Rakyat (Prosperous Justice Party Faction)</t>
         </is>
       </c>
-      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -2176,20 +2361,25 @@
           <t>0f88baee9a332f64f7937e5312e35cb5</t>
         </is>
       </c>
-      <c r="I38" t="b">
-        <v>1</v>
-      </c>
-      <c r="J38" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J38" t="b">
+        <v>1</v>
       </c>
       <c r="K38" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L38" t="inlineStr">
+        <is>
           <t>Muslim: Politician, Muslim, male, born 1971-03-01, in  for Democratic Party, Muslim: Politician, Muslim, male, born 1970-08-12, MUSLIM, SHI, MM: Public figure: Member of Dewan Perwakilan Rakyat (Democrat Party Faction)</t>
         </is>
       </c>
-      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -2217,20 +2407,25 @@
           <t>3c9b8639a8a20115e92f2fbe3a431b1c</t>
         </is>
       </c>
-      <c r="I39" t="b">
-        <v>1</v>
-      </c>
-      <c r="J39" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J39" t="b">
+        <v>1</v>
       </c>
       <c r="K39" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L39" t="inlineStr">
+        <is>
           <t>Nasarudin: Politician, Nasarudin, male, born 1982-07-12 for Golongan Karya Party, Nasaruddin: Politician, Nasaruddin, male, born 1957-07-17 for Great Indonesia Movement Party, Nasrudin: Politician, Nasrudin, male, born 1957-05-24, in Brebes for Golongan Karya Party</t>
         </is>
       </c>
-      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -2258,20 +2453,25 @@
           <t>e22653d732bbb161423e30feeb73c7c6</t>
         </is>
       </c>
-      <c r="I40" t="b">
-        <v>1</v>
-      </c>
-      <c r="J40" t="inlineStr">
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J40" t="b">
+        <v>1</v>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K40" t="inlineStr">
+      <c r="L40" t="inlineStr">
         <is>
           <t>Mat Solar: Politician, Nasrullah, male, born 1962-12-04, in Jakarta for United Development Party, Nasrullah: Politician, Nasrullah, male, born 1968-11-18, in Pekalongan for National Mandate Party</t>
         </is>
       </c>
-      <c r="L40" t="inlineStr">
+      <c r="M40" t="inlineStr">
         <is>
           <t>Nasrullah KHAN: Court: Manchester;
 Offence: Drugs Class A;
@@ -2312,20 +2512,25 @@
           <t>114f5e1c2da5c4152d0e07747b51176e</t>
         </is>
       </c>
-      <c r="I41" t="b">
-        <v>1</v>
-      </c>
-      <c r="J41" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J41" t="b">
+        <v>1</v>
       </c>
       <c r="K41" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L41" t="inlineStr">
+        <is>
           <t>Nur'aeni: Politician, Nur'aeni, female, born 1974-10-05 for Democratic Party, Nuraini: Politician, Nuraini, female, born 1973-06-10 for Indonesian Democratic Party – Struggle, Nuraini: Politician, Nuraini, female, born 1989-01-13 for National Awakening Party</t>
         </is>
       </c>
-      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -2353,20 +2558,25 @@
           <t>4344af06e3012e88d01cc66c2ebf46e8</t>
         </is>
       </c>
-      <c r="I42" t="b">
-        <v>1</v>
-      </c>
-      <c r="J42" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J42" t="b">
+        <v>1</v>
       </c>
       <c r="K42" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
           <t>Nuraini: Politician, Nuraini, female, born 1973-06-10 for Indonesian Democratic Party – Struggle, Nuraini: Politician, Nuraini, female, born 1989-01-13 for National Awakening Party, Nur'aeni: Politician, Nur'aeni, female, born 1974-10-05 for Democratic Party</t>
         </is>
       </c>
-      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -2394,20 +2604,25 @@
           <t>f4497340d6727ba20c13dfc2c2ae4cce</t>
         </is>
       </c>
-      <c r="I43" t="b">
-        <v>1</v>
-      </c>
-      <c r="J43" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J43" t="b">
+        <v>1</v>
       </c>
       <c r="K43" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
           <t>Nuryati: Politician, Nuryati, female, born 1975-03-01 for Prosperous Justice Party, Nurhayati: Politician, Nurhayati, female, born 1969-11-20, in Tasikmalaya for United Development Party, Hj. NURHAYATI: Public figure: Member of Dewan Perwakilan Rakyat (United Development Party Faction)</t>
         </is>
       </c>
-      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -2435,20 +2650,25 @@
           <t>478a62f94308d8ad5efca6fadd751936</t>
         </is>
       </c>
-      <c r="I44" t="b">
-        <v>1</v>
-      </c>
-      <c r="J44" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J44" t="b">
+        <v>1</v>
       </c>
       <c r="K44" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L44" t="inlineStr">
+        <is>
           <t>Suhardi: Deceased 2014-08-28, Suhardiman: Deceased 2015-12-13, Suharto: Deceased 2008-01-27</t>
         </is>
       </c>
-      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -2476,20 +2696,25 @@
           <t>964921fb11dc4b233ab661c98507c8d5</t>
         </is>
       </c>
-      <c r="I45" t="b">
-        <v>1</v>
-      </c>
-      <c r="J45" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J45" t="b">
+        <v>1</v>
       </c>
       <c r="K45" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L45" t="inlineStr">
+        <is>
           <t>Amiruddin: Politician, Amiruddin, male, born 1951-11-10 for Democratic Party, Amirudin: Politician, Amirudin, male, born 1971-12-13</t>
         </is>
       </c>
-      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -2517,20 +2742,25 @@
           <t>8ac10a93bb281087af272b8776b496e7</t>
         </is>
       </c>
-      <c r="I46" t="b">
-        <v>1</v>
-      </c>
-      <c r="J46" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J46" t="b">
+        <v>1</v>
       </c>
       <c r="K46" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L46" t="inlineStr">
+        <is>
           <t>Usman Khan: Politician, Usman Khan, male, born 1947-09-01, in  for Pakistan Tehreek-e-Insaf, Usmandy S: Politician, Usmandy S, male, born 1966-03-27</t>
         </is>
       </c>
-      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -2558,20 +2788,25 @@
           <t>646925253b92d8f15238c9f55a944bb2</t>
         </is>
       </c>
-      <c r="I47" t="b">
-        <v>1</v>
-      </c>
-      <c r="J47" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J47" t="b">
+        <v>1</v>
       </c>
       <c r="K47" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L47" t="inlineStr">
+        <is>
           <t>Muhammad Hamza: Deceased 2021-08-29, T. K. Hamza: Foreigner: India; Dominion of India; British Raj</t>
         </is>
       </c>
-      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -2599,20 +2834,25 @@
           <t>b3baf07134e501694ab06d4dafe4b8d9</t>
         </is>
       </c>
-      <c r="I48" t="b">
-        <v>1</v>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J48" t="b">
+        <v>1</v>
       </c>
       <c r="K48" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L48" t="inlineStr">
+        <is>
           <t>Muhammad Hamza: Deceased 2021-08-29, T. K. Hamza: Foreigner: India; Dominion of India; British Raj</t>
         </is>
       </c>
-      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -2645,20 +2885,25 @@
           <t>af1cb60ea9e8d6996c486b4370a8f294</t>
         </is>
       </c>
-      <c r="I49" t="b">
-        <v>1</v>
-      </c>
-      <c r="J49" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J49" t="b">
+        <v>1</v>
       </c>
       <c r="K49" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L49" t="inlineStr">
+        <is>
           <t>Usman Ibrahim: Foreigner: Pakistan; British Raj, Usman Ibrahim: Foreigner: Pakistan; British India</t>
         </is>
       </c>
-      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -2686,20 +2931,25 @@
           <t>6799749275c6b961b7412fb240c668d4</t>
         </is>
       </c>
-      <c r="I50" t="b">
-        <v>1</v>
-      </c>
-      <c r="J50" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J50" t="b">
+        <v>1</v>
       </c>
       <c r="K50" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L50" t="inlineStr">
+        <is>
           <t>Ilham: Politician, Ilham, male, born 1975-05-08, Ilham: Politician, Ilham, male, born 1968-09-08</t>
         </is>
       </c>
-      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -2727,20 +2977,25 @@
           <t>0d1e7cb998cad916cfec64bd72107ff4</t>
         </is>
       </c>
-      <c r="I51" t="b">
-        <v>1</v>
-      </c>
-      <c r="J51" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>2023-07-01</t>
+        </is>
+      </c>
+      <c r="J51" t="b">
+        <v>1</v>
       </c>
       <c r="K51" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L51" t="inlineStr">
+        <is>
           <t>Iwansyah: Politician, Iwansyah, male, born 1959-07-09, A. R. Iwansyah: Politician, A. R. Iwansyah, male, born 1960-08-11</t>
         </is>
       </c>
-      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -2768,20 +3023,25 @@
           <t>2a2ab1153cc82f221591b6f0c14c3780</t>
         </is>
       </c>
-      <c r="I52" t="b">
-        <v>1</v>
-      </c>
-      <c r="J52" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J52" t="b">
+        <v>1</v>
       </c>
       <c r="K52" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L52" t="inlineStr">
+        <is>
           <t>Mohammad Ali Jafari Brigadier Commander: Not an Indonesian name: محمد علي جعفري, Sayed Jafar: Politician, Sayed Jafar, male, born 1962-03-17</t>
         </is>
       </c>
-      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -2814,20 +3074,25 @@
           <t>ed15a8df79a7f97188cd2e2386f05dc2</t>
         </is>
       </c>
-      <c r="I53" t="b">
-        <v>1</v>
-      </c>
-      <c r="J53" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J53" t="b">
+        <v>1</v>
       </c>
       <c r="K53" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L53" t="inlineStr">
+        <is>
           <t>Ali Barakat: Not an Indonesian name: علي بركات, Ali: Politician, Ali, male, born 1950-09-01</t>
         </is>
       </c>
-      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -2860,20 +3125,25 @@
           <t>6e2f300824d953c6efc018a2267b9430</t>
         </is>
       </c>
-      <c r="I54" t="b">
-        <v>1</v>
-      </c>
-      <c r="J54" t="inlineStr">
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J54" t="b">
+        <v>1</v>
+      </c>
+      <c r="K54" t="inlineStr">
         <is>
           <t>Needs explanation</t>
         </is>
       </c>
-      <c r="K54" t="inlineStr">
+      <c r="L54" t="inlineStr">
         <is>
           <t>Dilip Kumar: Deceased 2021-07-07</t>
         </is>
       </c>
-      <c r="L54" t="inlineStr">
+      <c r="M54" t="inlineStr">
         <is>
           <t>'Abd al-Rahman Khalaf 'Ubayd Juday' AL-'ANIZI: 'Abd al-Rahman Khalaf AL-'ANZI, AL-RAHMAN, Abu Usamah, ABU USAMA, YUSUF, 'Abd al-Rahman Khalaf AL-ANIZI, KUWAITI, Abu Shaima', AL-KUWAITI, Abu Usamah, born 01 Jan 1973 to 31 Dec 1973</t>
         </is>
@@ -2905,20 +3175,25 @@
           <t>4dd814f0f0feb45f36d2818f5af11b65</t>
         </is>
       </c>
-      <c r="I55" t="b">
-        <v>1</v>
-      </c>
-      <c r="J55" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J55" t="b">
+        <v>1</v>
       </c>
       <c r="K55" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
           <t>M. Amin: Politician, M. Amin, male, born 1965-09-26, Amin Ak: Politician, Amin, male, born 1965-07-06 for Prosperous Justice Party</t>
         </is>
       </c>
-      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -2946,20 +3221,25 @@
           <t>1882d799e6f76da0fb227f294497edf4</t>
         </is>
       </c>
-      <c r="I56" t="b">
-        <v>1</v>
-      </c>
-      <c r="J56" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J56" t="b">
+        <v>1</v>
       </c>
       <c r="K56" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L56" t="inlineStr">
+        <is>
           <t>Kh. M. Mansyur: Politician, Kh. M. Mansyur, male, born 1947-06-10, Mansour Fadlallah Azzam: Not an Indonesian name: منصور فضل الله عزام</t>
         </is>
       </c>
-      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -2987,20 +3267,25 @@
           <t>0e848cb4bef0c25bfb158427bf81dcc4</t>
         </is>
       </c>
-      <c r="I57" t="b">
-        <v>1</v>
-      </c>
-      <c r="J57" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J57" t="b">
+        <v>1</v>
       </c>
       <c r="K57" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L57" t="inlineStr">
+        <is>
           <t>Nurhasanah: Politician, Nurhasanah, female, born 1957-02-22 for Democratic Party, Norhasanah: Politician, Norhasanah, female, born 1962-11-09, in Martapura for United Development Party</t>
         </is>
       </c>
-      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -3028,20 +3313,25 @@
           <t>a35809b6446be02f2f8c431397051db8</t>
         </is>
       </c>
-      <c r="I58" t="b">
-        <v>1</v>
-      </c>
-      <c r="J58" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J58" t="b">
+        <v>1</v>
       </c>
       <c r="K58" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
           <t>Salahudin: Politician, Salahudin, male, born 1969-10-12, Sheikh Salahuddin: Politician, Sheikh Salahuddin, male, born 1956-08-20 for Muttahida Qaumi Movement</t>
         </is>
       </c>
-      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -3069,20 +3359,25 @@
           <t>c8be3a4143a7a6bd5ce7fcb6a87fc83a</t>
         </is>
       </c>
-      <c r="I59" t="b">
-        <v>1</v>
-      </c>
-      <c r="J59" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J59" t="b">
+        <v>1</v>
       </c>
       <c r="K59" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
           <t>Syamsurizal: Politician, Syamsurizal, male, born 1955-06-25 for United Development Party, Samsuri: Politician, Samsuri, male, born 1952-04-20</t>
         </is>
       </c>
-      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -3110,20 +3405,25 @@
           <t>dccc003b931eacc48767ea3964855203</t>
         </is>
       </c>
-      <c r="I60" t="b">
-        <v>1</v>
-      </c>
-      <c r="J60" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J60" t="b">
+        <v>1</v>
       </c>
       <c r="K60" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
           <t>Syarifuddin: Politician, Syarifuddin, male, born 1965-10-19, Muhammad Syarifuddin: Politician, M. Syarifuddin, male, born 1954-10-17, in Baturaja</t>
         </is>
       </c>
-      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -3156,20 +3456,25 @@
           <t>4c7fc8fdd96caab1ddf8de3ed851f036</t>
         </is>
       </c>
-      <c r="I61" t="b">
-        <v>1</v>
-      </c>
-      <c r="J61" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J61" t="b">
+        <v>1</v>
       </c>
       <c r="K61" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
           <t>Siti Nurbaya Bakar: Politician, Siti Nurbaya, Dr. Ir. Siti Nurbaya Bakar, M.Sc., female, born 1956-08-28, in Jakarta for Nasdem Party, SITI Nurbaya Bakar: Public figure: Min. of Environment &amp; Forestry</t>
         </is>
       </c>
-      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -3202,20 +3507,25 @@
           <t>0cb9f03a5a5a4d34c6e6bfdb14dd9897</t>
         </is>
       </c>
-      <c r="I62" t="b">
-        <v>1</v>
-      </c>
-      <c r="J62" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I62" t="inlineStr">
+        <is>
+          <t>2023-07-06</t>
+        </is>
+      </c>
+      <c r="J62" t="b">
+        <v>1</v>
       </c>
       <c r="K62" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
           <t>Siti Nurbaya Bakar: Politician, Siti Nurbaya, Dr. Ir. Siti Nurbaya Bakar, M.Sc., female, born 1956-08-28, in Jakarta for Nasdem Party, SITI Nurbaya Bakar: Public figure: Min. of Environment &amp; Forestry</t>
         </is>
       </c>
-      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -3248,16 +3558,21 @@
           <t>31dbe3978f8046345248eb7b3e07513b</t>
         </is>
       </c>
-      <c r="I63" t="b">
+      <c r="I63" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J63" t="b">
         <v>0</v>
       </c>
-      <c r="J63" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
-      </c>
-      <c r="K63" t="inlineStr"/>
+      <c r="K63" t="inlineStr">
+        <is>
+          <t>False positive</t>
+        </is>
+      </c>
       <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -3285,20 +3600,25 @@
           <t>009de2b69f221ae3b8a85a65958e8a53</t>
         </is>
       </c>
-      <c r="I64" t="b">
-        <v>1</v>
-      </c>
-      <c r="J64" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I64" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J64" t="b">
+        <v>1</v>
       </c>
       <c r="K64" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
           <t>Suhardiman: Deceased 2015-12-13, Suhardi: Deceased 2014-08-28</t>
         </is>
       </c>
-      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -3326,20 +3646,25 @@
           <t>efa5293f0804df33929996ecc61a56a2</t>
         </is>
       </c>
-      <c r="I65" t="b">
-        <v>1</v>
-      </c>
-      <c r="J65" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I65" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J65" t="b">
+        <v>1</v>
       </c>
       <c r="K65" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
           <t>Sunardi: Politician, Sunardi, male, born 1966-12-05 for Prosperous Justice Party, Sunardi: Politician, Sunardi, male, born 1948-02-09</t>
         </is>
       </c>
-      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -3367,20 +3692,25 @@
           <t>26613526b2542e9297e387d0130b8f50</t>
         </is>
       </c>
-      <c r="I66" t="b">
-        <v>1</v>
-      </c>
-      <c r="J66" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I66" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J66" t="b">
+        <v>1</v>
       </c>
       <c r="K66" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
           <t>Supratman: Politician, Supratman, male, born 1959-05-04, in Medan for Indonesian Justice and Unity Party, Supratman: Politician, Supratman, male, born 1949-10-05</t>
         </is>
       </c>
-      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -3408,20 +3738,25 @@
           <t>54369dd59db8d12945cd550c215bc52b</t>
         </is>
       </c>
-      <c r="I67" t="b">
-        <v>1</v>
-      </c>
-      <c r="J67" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I67" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J67" t="b">
+        <v>1</v>
       </c>
       <c r="K67" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
           <t>Supriadi: Politician, Supriadi, male, born 1968-08-08, Supriadi: Politician, Supriadi, male, born 1968-01-04</t>
         </is>
       </c>
-      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -3449,20 +3784,25 @@
           <t>f5d0c4d081d11da1d03355577bdc0f39</t>
         </is>
       </c>
-      <c r="I68" t="b">
-        <v>1</v>
-      </c>
-      <c r="J68" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I68" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J68" t="b">
+        <v>1</v>
       </c>
       <c r="K68" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
           <t>Syafrudin: Politician, Syafrudin, male, born 1958-08-10 for Nasdem Party, Syafruddin: Politician, Syafruddin, male, born 1958-07-20</t>
         </is>
       </c>
-      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -3490,20 +3830,25 @@
           <t>95bd94215021d01aa50a6d1d36d52bb8</t>
         </is>
       </c>
-      <c r="I69" t="b">
-        <v>1</v>
-      </c>
-      <c r="J69" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I69" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J69" t="b">
+        <v>1</v>
       </c>
       <c r="K69" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
           <t>Syamsurizal: Politician, Syamsurizal, male, born 1955-06-25 for United Development Party, Samsuri: Politician, Samsuri, male, born 1952-04-20</t>
         </is>
       </c>
-      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -3531,20 +3876,25 @@
           <t>b73ac6e560549a0bb0577f5a9d0b349a</t>
         </is>
       </c>
-      <c r="I70" t="b">
-        <v>1</v>
-      </c>
-      <c r="J70" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I70" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J70" t="b">
+        <v>1</v>
       </c>
       <c r="K70" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
           <t>Usman Khan: Politician, Usman Khan, male, born 1947-09-01, in  for Pakistan Tehreek-e-Insaf, Usmandy S: Politician, Usmandy S, male, born 1966-03-27</t>
         </is>
       </c>
-      <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -3572,20 +3922,25 @@
           <t>d0b5926c4a23d89cd1ef902c223b9b83</t>
         </is>
       </c>
-      <c r="I71" t="b">
-        <v>1</v>
-      </c>
-      <c r="J71" t="inlineStr">
-        <is>
-          <t>False positive</t>
-        </is>
+      <c r="I71" t="inlineStr">
+        <is>
+          <t>2023-07-09</t>
+        </is>
+      </c>
+      <c r="J71" t="b">
+        <v>1</v>
       </c>
       <c r="K71" t="inlineStr">
         <is>
+          <t>False positive</t>
+        </is>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
           <t>M. Amin: Politician, M. Amin, male, born 1965-09-26, Amin Ak: Politician, Amin, male, born 1965-07-06 for Prosperous Justice Party</t>
         </is>
       </c>
-      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Convert xlsx to CSV
to ensure that all values are cast to string

branch:
</commit_message>
<xml_diff>
--- a/tests/test_resources/test_namescan_explained.xlsx
+++ b/tests/test_resources/test_namescan_explained.xlsx
@@ -499,6 +499,7 @@
           <t>Muhammad</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr"/>
       <c r="D2" t="inlineStr">
         <is>
           <t>Ali</t>
@@ -509,6 +510,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F2" t="inlineStr"/>
       <c r="G2" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -567,11 +569,14 @@
           <t>Muhammad</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr"/>
+      <c r="D3" t="inlineStr"/>
       <c r="E3" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F3" t="inlineStr"/>
       <c r="G3" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -613,6 +618,7 @@
           <t>Abdul</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr"/>
       <c r="D4" t="inlineStr">
         <is>
           <t>Azis</t>
@@ -623,6 +629,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F4" t="inlineStr"/>
       <c r="G4" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -677,11 +684,14 @@
           <t>H. Abdullah</t>
         </is>
       </c>
+      <c r="C5" t="inlineStr"/>
+      <c r="D5" t="inlineStr"/>
       <c r="E5" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F5" t="inlineStr"/>
       <c r="G5" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -738,6 +748,7 @@
           <t>Abu</t>
         </is>
       </c>
+      <c r="C6" t="inlineStr"/>
       <c r="D6" t="inlineStr">
         <is>
           <t>Bakar</t>
@@ -748,6 +759,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F6" t="inlineStr"/>
       <c r="G6" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -796,11 +808,14 @@
           <t>Muhammadiyah</t>
         </is>
       </c>
+      <c r="C7" t="inlineStr"/>
+      <c r="D7" t="inlineStr"/>
       <c r="E7" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr"/>
       <c r="G7" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -842,11 +857,14 @@
           <t>H.Abdollah</t>
         </is>
       </c>
+      <c r="C8" t="inlineStr"/>
+      <c r="D8" t="inlineStr"/>
       <c r="E8" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F8" t="inlineStr"/>
       <c r="G8" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -892,11 +910,14 @@
           <t>Hasan</t>
         </is>
       </c>
+      <c r="C9" t="inlineStr"/>
+      <c r="D9" t="inlineStr"/>
       <c r="E9" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F9" t="inlineStr"/>
       <c r="G9" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -938,11 +959,14 @@
           <t>Ahmad</t>
         </is>
       </c>
+      <c r="C10" t="inlineStr"/>
+      <c r="D10" t="inlineStr"/>
       <c r="E10" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F10" t="inlineStr"/>
       <c r="G10" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1003,6 +1027,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F11" t="inlineStr"/>
       <c r="G11" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1044,11 +1069,14 @@
           <t>Mahmud</t>
         </is>
       </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
       <c r="E12" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F12" t="inlineStr"/>
       <c r="G12" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1103,6 +1131,7 @@
           <t>A.Hamid</t>
         </is>
       </c>
+      <c r="C13" t="inlineStr"/>
       <c r="D13" t="inlineStr">
         <is>
           <t>Ahmad</t>
@@ -1113,6 +1142,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F13" t="inlineStr"/>
       <c r="G13" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1158,11 +1188,14 @@
           <t>Abdurrahman</t>
         </is>
       </c>
+      <c r="C14" t="inlineStr"/>
+      <c r="D14" t="inlineStr"/>
       <c r="E14" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F14" t="inlineStr"/>
       <c r="G14" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1210,6 +1243,7 @@
           <t>Muhammad</t>
         </is>
       </c>
+      <c r="C15" t="inlineStr"/>
       <c r="D15" t="inlineStr">
         <is>
           <t>Hatta</t>
@@ -1220,6 +1254,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F15" t="inlineStr"/>
       <c r="G15" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1261,6 +1296,7 @@
           <t>Abdul</t>
         </is>
       </c>
+      <c r="C16" t="inlineStr"/>
       <c r="D16" t="inlineStr">
         <is>
           <t>Gani</t>
@@ -1271,6 +1307,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F16" t="inlineStr"/>
       <c r="G16" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1312,6 +1349,7 @@
           <t>Ahmad</t>
         </is>
       </c>
+      <c r="C17" t="inlineStr"/>
       <c r="D17" t="inlineStr">
         <is>
           <t>Hasan</t>
@@ -1322,6 +1360,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F17" t="inlineStr"/>
       <c r="G17" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1363,6 +1402,7 @@
           <t>Ibrahim</t>
         </is>
       </c>
+      <c r="C18" t="inlineStr"/>
       <c r="D18" t="inlineStr">
         <is>
           <t>Hasan</t>
@@ -1373,6 +1413,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F18" t="inlineStr"/>
       <c r="G18" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1414,11 +1455,14 @@
           <t>Mulyadi</t>
         </is>
       </c>
+      <c r="C19" t="inlineStr"/>
+      <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F19" t="inlineStr"/>
       <c r="G19" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1460,11 +1504,14 @@
           <t>Ismail</t>
         </is>
       </c>
+      <c r="C20" t="inlineStr"/>
+      <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F20" t="inlineStr"/>
       <c r="G20" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1506,11 +1553,14 @@
           <t>M.Ali</t>
         </is>
       </c>
+      <c r="C21" t="inlineStr"/>
+      <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F21" t="inlineStr"/>
       <c r="G21" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1556,11 +1606,14 @@
           <t>Muh.Ali</t>
         </is>
       </c>
+      <c r="C22" t="inlineStr"/>
+      <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F22" t="inlineStr"/>
       <c r="G22" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1606,11 +1659,14 @@
           <t>Nasrullah</t>
         </is>
       </c>
+      <c r="C23" t="inlineStr"/>
+      <c r="D23" t="inlineStr"/>
       <c r="E23" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F23" t="inlineStr"/>
       <c r="G23" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1665,11 +1721,14 @@
           <t>Rahman</t>
         </is>
       </c>
+      <c r="C24" t="inlineStr"/>
+      <c r="D24" t="inlineStr"/>
       <c r="E24" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F24" t="inlineStr"/>
       <c r="G24" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1718,11 +1777,14 @@
           <t>Anwar</t>
         </is>
       </c>
+      <c r="C25" t="inlineStr"/>
+      <c r="D25" t="inlineStr"/>
       <c r="E25" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F25" t="inlineStr"/>
       <c r="G25" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1770,11 +1832,14 @@
           <t>Ibrahim</t>
         </is>
       </c>
+      <c r="C26" t="inlineStr"/>
+      <c r="D26" t="inlineStr"/>
       <c r="E26" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F26" t="inlineStr"/>
       <c r="G26" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1816,11 +1881,14 @@
           <t>Samsudin</t>
         </is>
       </c>
+      <c r="C27" t="inlineStr"/>
+      <c r="D27" t="inlineStr"/>
       <c r="E27" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F27" t="inlineStr"/>
       <c r="G27" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1862,11 +1930,14 @@
           <t>Sudirman</t>
         </is>
       </c>
+      <c r="C28" t="inlineStr"/>
+      <c r="D28" t="inlineStr"/>
       <c r="E28" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F28" t="inlineStr"/>
       <c r="G28" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1908,11 +1979,14 @@
           <t>Sukiman</t>
         </is>
       </c>
+      <c r="C29" t="inlineStr"/>
+      <c r="D29" t="inlineStr"/>
       <c r="E29" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F29" t="inlineStr"/>
       <c r="G29" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -1954,11 +2028,14 @@
           <t>Syamsudin</t>
         </is>
       </c>
+      <c r="C30" t="inlineStr"/>
+      <c r="D30" t="inlineStr"/>
       <c r="E30" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F30" t="inlineStr"/>
       <c r="G30" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2000,6 +2077,7 @@
           <t>Abdul</t>
         </is>
       </c>
+      <c r="C31" t="inlineStr"/>
       <c r="D31" t="inlineStr">
         <is>
           <t>Haris</t>
@@ -2010,6 +2088,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F31" t="inlineStr"/>
       <c r="G31" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2066,6 +2145,7 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="F32" t="inlineStr"/>
       <c r="G32" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2111,11 +2191,14 @@
           <t>Firman</t>
         </is>
       </c>
+      <c r="C33" t="inlineStr"/>
+      <c r="D33" t="inlineStr"/>
       <c r="E33" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F33" t="inlineStr"/>
       <c r="G33" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2157,11 +2240,14 @@
           <t>Haerudin</t>
         </is>
       </c>
+      <c r="C34" t="inlineStr"/>
+      <c r="D34" t="inlineStr"/>
       <c r="E34" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F34" t="inlineStr"/>
       <c r="G34" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2203,11 +2289,14 @@
           <t>Imran</t>
         </is>
       </c>
+      <c r="C35" t="inlineStr"/>
+      <c r="D35" t="inlineStr"/>
       <c r="E35" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F35" t="inlineStr"/>
       <c r="G35" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2249,6 +2338,7 @@
           <t>M</t>
         </is>
       </c>
+      <c r="C36" t="inlineStr"/>
       <c r="D36" t="inlineStr">
         <is>
           <t>Nasir</t>
@@ -2259,6 +2349,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F36" t="inlineStr"/>
       <c r="G36" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2300,11 +2391,14 @@
           <t>Murdani</t>
         </is>
       </c>
+      <c r="C37" t="inlineStr"/>
+      <c r="D37" t="inlineStr"/>
       <c r="E37" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F37" t="inlineStr"/>
       <c r="G37" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2346,11 +2440,14 @@
           <t>Muslim</t>
         </is>
       </c>
+      <c r="C38" t="inlineStr"/>
+      <c r="D38" t="inlineStr"/>
       <c r="E38" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F38" t="inlineStr"/>
       <c r="G38" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2392,11 +2489,14 @@
           <t>Nasarudin</t>
         </is>
       </c>
+      <c r="C39" t="inlineStr"/>
+      <c r="D39" t="inlineStr"/>
       <c r="E39" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F39" t="inlineStr"/>
       <c r="G39" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2438,11 +2538,14 @@
           <t>Nasarullah</t>
         </is>
       </c>
+      <c r="C40" t="inlineStr"/>
+      <c r="D40" t="inlineStr"/>
       <c r="E40" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F40" t="inlineStr"/>
       <c r="G40" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2497,11 +2600,14 @@
           <t>Nuraeni</t>
         </is>
       </c>
+      <c r="C41" t="inlineStr"/>
+      <c r="D41" t="inlineStr"/>
       <c r="E41" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
+      <c r="F41" t="inlineStr"/>
       <c r="G41" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2543,11 +2649,14 @@
           <t>Nuraini</t>
         </is>
       </c>
+      <c r="C42" t="inlineStr"/>
+      <c r="D42" t="inlineStr"/>
       <c r="E42" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
+      <c r="F42" t="inlineStr"/>
       <c r="G42" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2589,11 +2698,14 @@
           <t>Nurati</t>
         </is>
       </c>
+      <c r="C43" t="inlineStr"/>
+      <c r="D43" t="inlineStr"/>
       <c r="E43" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
+      <c r="F43" t="inlineStr"/>
       <c r="G43" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2635,11 +2747,14 @@
           <t>Suhardin</t>
         </is>
       </c>
+      <c r="C44" t="inlineStr"/>
+      <c r="D44" t="inlineStr"/>
       <c r="E44" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F44" t="inlineStr"/>
       <c r="G44" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2681,11 +2796,14 @@
           <t>Amiruddin</t>
         </is>
       </c>
+      <c r="C45" t="inlineStr"/>
+      <c r="D45" t="inlineStr"/>
       <c r="E45" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F45" t="inlineStr"/>
       <c r="G45" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2727,11 +2845,14 @@
           <t>H.Usman</t>
         </is>
       </c>
+      <c r="C46" t="inlineStr"/>
+      <c r="D46" t="inlineStr"/>
       <c r="E46" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F46" t="inlineStr"/>
       <c r="G46" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2773,11 +2894,14 @@
           <t>H.Hamzah</t>
         </is>
       </c>
+      <c r="C47" t="inlineStr"/>
+      <c r="D47" t="inlineStr"/>
       <c r="E47" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F47" t="inlineStr"/>
       <c r="G47" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2819,11 +2943,14 @@
           <t>Hamzah</t>
         </is>
       </c>
+      <c r="C48" t="inlineStr"/>
+      <c r="D48" t="inlineStr"/>
       <c r="E48" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F48" t="inlineStr"/>
       <c r="G48" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2865,6 +2992,7 @@
           <t>Ibrahim</t>
         </is>
       </c>
+      <c r="C49" t="inlineStr"/>
       <c r="D49" t="inlineStr">
         <is>
           <t>Usman</t>
@@ -2875,6 +3003,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F49" t="inlineStr"/>
       <c r="G49" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2916,11 +3045,14 @@
           <t>Ilham</t>
         </is>
       </c>
+      <c r="C50" t="inlineStr"/>
+      <c r="D50" t="inlineStr"/>
       <c r="E50" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F50" t="inlineStr"/>
       <c r="G50" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -2962,11 +3094,14 @@
           <t>Iwansyah</t>
         </is>
       </c>
+      <c r="C51" t="inlineStr"/>
+      <c r="D51" t="inlineStr"/>
       <c r="E51" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F51" t="inlineStr"/>
       <c r="G51" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3008,11 +3143,14 @@
           <t>Jafar</t>
         </is>
       </c>
+      <c r="C52" t="inlineStr"/>
+      <c r="D52" t="inlineStr"/>
       <c r="E52" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F52" t="inlineStr"/>
       <c r="G52" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3054,6 +3192,7 @@
           <t>M</t>
         </is>
       </c>
+      <c r="C53" t="inlineStr"/>
       <c r="D53" t="inlineStr">
         <is>
           <t>Ali</t>
@@ -3064,6 +3203,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F53" t="inlineStr"/>
       <c r="G53" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3105,6 +3245,7 @@
           <t>M</t>
         </is>
       </c>
+      <c r="C54" t="inlineStr"/>
       <c r="D54" t="inlineStr">
         <is>
           <t>Yusuf</t>
@@ -3115,6 +3256,7 @@
           <t>Male</t>
         </is>
       </c>
+      <c r="F54" t="inlineStr"/>
       <c r="G54" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3160,11 +3302,14 @@
           <t>M.Amin</t>
         </is>
       </c>
+      <c r="C55" t="inlineStr"/>
+      <c r="D55" t="inlineStr"/>
       <c r="E55" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F55" t="inlineStr"/>
       <c r="G55" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3206,11 +3351,14 @@
           <t>Mansyur</t>
         </is>
       </c>
+      <c r="C56" t="inlineStr"/>
+      <c r="D56" t="inlineStr"/>
       <c r="E56" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F56" t="inlineStr"/>
       <c r="G56" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3252,11 +3400,14 @@
           <t>Nurhasanah</t>
         </is>
       </c>
+      <c r="C57" t="inlineStr"/>
+      <c r="D57" t="inlineStr"/>
       <c r="E57" t="inlineStr">
         <is>
           <t>Female</t>
         </is>
       </c>
+      <c r="F57" t="inlineStr"/>
       <c r="G57" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3298,11 +3449,14 @@
           <t>Salahuddin</t>
         </is>
       </c>
+      <c r="C58" t="inlineStr"/>
+      <c r="D58" t="inlineStr"/>
       <c r="E58" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F58" t="inlineStr"/>
       <c r="G58" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3344,11 +3498,14 @@
           <t>Samsurizal</t>
         </is>
       </c>
+      <c r="C59" t="inlineStr"/>
+      <c r="D59" t="inlineStr"/>
       <c r="E59" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F59" t="inlineStr"/>
       <c r="G59" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3390,11 +3547,14 @@
           <t>Syarifudin</t>
         </is>
       </c>
+      <c r="C60" t="inlineStr"/>
+      <c r="D60" t="inlineStr"/>
       <c r="E60" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F60" t="inlineStr"/>
       <c r="G60" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3436,6 +3596,7 @@
           <t>Siti</t>
         </is>
       </c>
+      <c r="C61" t="inlineStr"/>
       <c r="D61" t="inlineStr">
         <is>
           <t>Nurbaya</t>
@@ -3446,6 +3607,7 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="F61" t="inlineStr"/>
       <c r="G61" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3487,6 +3649,7 @@
           <t>Sitti</t>
         </is>
       </c>
+      <c r="C62" t="inlineStr"/>
       <c r="D62" t="inlineStr">
         <is>
           <t>Nurbaya</t>
@@ -3497,6 +3660,7 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="F62" t="inlineStr"/>
       <c r="G62" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3538,6 +3702,7 @@
           <t>Sitti</t>
         </is>
       </c>
+      <c r="C63" t="inlineStr"/>
       <c r="D63" t="inlineStr">
         <is>
           <t>Nurbaya</t>
@@ -3548,6 +3713,7 @@
           <t>Female</t>
         </is>
       </c>
+      <c r="F63" t="inlineStr"/>
       <c r="G63" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3585,11 +3751,14 @@
           <t>Suhardiman</t>
         </is>
       </c>
+      <c r="C64" t="inlineStr"/>
+      <c r="D64" t="inlineStr"/>
       <c r="E64" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F64" t="inlineStr"/>
       <c r="G64" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3631,11 +3800,14 @@
           <t>Sunardin</t>
         </is>
       </c>
+      <c r="C65" t="inlineStr"/>
+      <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F65" t="inlineStr"/>
       <c r="G65" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3677,11 +3849,14 @@
           <t>Supratman</t>
         </is>
       </c>
+      <c r="C66" t="inlineStr"/>
+      <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F66" t="inlineStr"/>
       <c r="G66" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3723,11 +3898,14 @@
           <t>Supriadin</t>
         </is>
       </c>
+      <c r="C67" t="inlineStr"/>
+      <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F67" t="inlineStr"/>
       <c r="G67" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3769,11 +3947,14 @@
           <t>Syafrudin</t>
         </is>
       </c>
+      <c r="C68" t="inlineStr"/>
+      <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F68" t="inlineStr"/>
       <c r="G68" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3815,11 +3996,14 @@
           <t>Syamsurizal</t>
         </is>
       </c>
+      <c r="C69" t="inlineStr"/>
+      <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F69" t="inlineStr"/>
       <c r="G69" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3861,11 +4045,14 @@
           <t>Usman</t>
         </is>
       </c>
+      <c r="C70" t="inlineStr"/>
+      <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F70" t="inlineStr"/>
       <c r="G70" t="inlineStr">
         <is>
           <t>Indonesia</t>
@@ -3907,11 +4094,14 @@
           <t>Yamin</t>
         </is>
       </c>
+      <c r="C71" t="inlineStr"/>
+      <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr">
         <is>
           <t>Male</t>
         </is>
       </c>
+      <c r="F71" t="inlineStr"/>
       <c r="G71" t="inlineStr">
         <is>
           <t>Indonesia</t>

</xml_diff>